<commit_message>
finish group by job
</commit_message>
<xml_diff>
--- a/party/20251014一条.xlsx
+++ b/party/20251014一条.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4500" yWindow="4010" windowWidth="28800" windowHeight="15460" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,19 +16,26 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -452,24 +459,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col width="14.1796875" customWidth="1" min="1" max="1"/>
-    <col width="34.26953125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="37.54296875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="56.6328125" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="60.6328125" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="11.7265625" customWidth="1" min="6" max="6"/>
-    <col width="16.7265625" customWidth="1" min="7" max="7"/>
+    <col width="20.58203125" customWidth="1" min="1" max="15"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.5" customHeight="1">
+    <row r="1" ht="22.5" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>奶</t>
@@ -477,91 +478,199 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>圣骑</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>拳</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>弩</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>船</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>饺子</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>刀</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>弓</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>标</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>火毒</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>单挂</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="n"/>
+      <c r="O1" s="1" t="n"/>
+    </row>
+    <row r="2" ht="22.5" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
           <t>义气丶奶</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>森贝尔嫩</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>章章浩</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>阿树</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>点恋线</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>朗姆</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>浪客阿文</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>滴滴叭叭</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>枇杷树</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>喃</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>猫猫爱金币</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>4. 柠檬-105勇士 求母本</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="n"/>
+      <c r="N2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+    </row>
+    <row r="3" ht="22.5" customHeight="1">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>as</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>声微饭否</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>日落沙滩前</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>莉莎长高高</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="n"/>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>穷到捡破烂</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>厉飞羽</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>Cris</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>Nemo尼莫</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>timemei</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="n"/>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>6. 给糖就约-140龙骑 单挂</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="n"/>
+      <c r="N3" s="1" t="n"/>
+      <c r="O3" s="1" t="n"/>
+    </row>
+    <row r="4" ht="22.5" customHeight="1">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>千万恶霸</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>战斗猫</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
-    </row>
-    <row r="2" ht="23.5" customHeight="1">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>火</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>森贝尔嫩</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>声微饭否</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>强人锁男</t>
         </is>
       </c>
-      <c r="E2" s="1" t="n"/>
-      <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
-    </row>
-    <row r="3" ht="23.5" customHeight="1">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>圣骑</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>章章浩</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>日落沙滩前</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>一天也</t>
-        </is>
-      </c>
-      <c r="E3" s="1" t="n"/>
-      <c r="F3" s="1" t="n"/>
-      <c r="G3" s="1" t="n"/>
-    </row>
-    <row r="4" ht="23.5" customHeight="1">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>拳</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>阿树</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>莉莎长高高</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
@@ -572,16 +681,40 @@
       <c r="E4" s="1" t="n"/>
       <c r="F4" s="1" t="n"/>
       <c r="G4" s="1" t="n"/>
-    </row>
-    <row r="5" ht="23.5" customHeight="1">
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>菜叶子</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t>鱼儿爱看雪</t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>纯白色</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="n"/>
+      <c r="L4" s="1" t="inlineStr">
+        <is>
+          <t>29. 倩倩子-120奶  单挂，需要一个杯子</t>
+        </is>
+      </c>
+      <c r="M4" s="1" t="n"/>
+      <c r="N4" s="1" t="n"/>
+      <c r="O4" s="1" t="n"/>
+    </row>
+    <row r="5" ht="22.5" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>弩</t>
+          <t>战斗猫</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>点恋线</t>
+          <t>冰峡江月</t>
         </is>
       </c>
       <c r="C5" s="1" t="n"/>
@@ -589,147 +722,135 @@
       <c r="E5" s="1" t="n"/>
       <c r="F5" s="1" t="n"/>
       <c r="G5" s="1" t="n"/>
-    </row>
-    <row r="6" ht="23.5" customHeight="1">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>船</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>朗姆</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>穷到捡破烂</t>
-        </is>
-      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>暗影灬</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="inlineStr">
+        <is>
+          <t>怪力</t>
+        </is>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>李蛋卷</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="n"/>
+      <c r="L5" s="1" t="inlineStr">
+        <is>
+          <t>33. 冰封de记忆 冰雷 单挂，需求扎头杯子</t>
+        </is>
+      </c>
+      <c r="M5" s="1" t="n"/>
+      <c r="N5" s="1" t="n"/>
+      <c r="O5" s="1" t="n"/>
+    </row>
+    <row r="6" ht="22.5" customHeight="1">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
       <c r="D6" s="1" t="n"/>
       <c r="E6" s="1" t="n"/>
       <c r="F6" s="1" t="n"/>
       <c r="G6" s="1" t="n"/>
-    </row>
-    <row r="7" ht="23.5" customHeight="1">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>饺子</t>
-        </is>
-      </c>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>浪客阿文</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>厉飞羽</t>
-        </is>
-      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>无敌铁锅</t>
+        </is>
+      </c>
+      <c r="I6" s="1" t="inlineStr">
+        <is>
+          <t>Hoyt</t>
+        </is>
+      </c>
+      <c r="J6" s="1" t="n"/>
+      <c r="K6" s="1" t="n"/>
+      <c r="L6" s="1" t="n"/>
+      <c r="M6" s="1" t="n"/>
+      <c r="N6" s="1" t="n"/>
+      <c r="O6" s="1" t="n"/>
+    </row>
+    <row r="7" ht="22.5" customHeight="1">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
       <c r="D7" s="1" t="n"/>
       <c r="E7" s="1" t="n"/>
       <c r="F7" s="1" t="n"/>
       <c r="G7" s="1" t="n"/>
-    </row>
-    <row r="8" ht="23.5" customHeight="1">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>刀</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>滴滴叭叭</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>Cris</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>菜叶子</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="inlineStr">
-        <is>
-          <t>暗影灬</t>
-        </is>
-      </c>
-      <c r="F8" s="1" t="inlineStr">
-        <is>
-          <t>无敌铁锅</t>
-        </is>
-      </c>
+      <c r="H7" s="1" t="inlineStr">
+        <is>
+          <t>Flash936</t>
+        </is>
+      </c>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
+          <t>与小女</t>
+        </is>
+      </c>
+      <c r="J7" s="1" t="n"/>
+      <c r="K7" s="1" t="n"/>
+      <c r="L7" s="1" t="n"/>
+      <c r="M7" s="1" t="n"/>
+      <c r="N7" s="1" t="n"/>
+      <c r="O7" s="1" t="n"/>
+    </row>
+    <row r="8" ht="22.5" customHeight="1">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="n"/>
+      <c r="F8" s="1" t="n"/>
       <c r="G8" s="1" t="n"/>
-    </row>
-    <row r="9" ht="23.5" customHeight="1">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>弓</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>枇杷树</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>Nemo尼莫</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>鱼儿爱看雪</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="inlineStr">
-        <is>
-          <t>怪力</t>
-        </is>
-      </c>
-      <c r="F9" s="1" t="inlineStr">
-        <is>
-          <t>Hoyt</t>
-        </is>
-      </c>
-      <c r="G9" s="1" t="inlineStr">
-        <is>
-          <t>与小女</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="23.5" customHeight="1">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>单挂</t>
-        </is>
-      </c>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>4. 柠檬-105勇士 求母本</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="inlineStr">
-        <is>
-          <t>6. 给糖就约-140龙骑 单挂</t>
-        </is>
-      </c>
-      <c r="D10" s="1" t="inlineStr">
-        <is>
-          <t>29. 倩倩子-120奶  单挂，需要一个杯子</t>
-        </is>
-      </c>
-      <c r="E10" s="1" t="inlineStr">
-        <is>
-          <t>33. 冰封de记忆 冰雷 单挂，需求扎头杯子</t>
-        </is>
-      </c>
+      <c r="H8" s="1" t="inlineStr">
+        <is>
+          <t>灰心</t>
+        </is>
+      </c>
+      <c r="I8" s="1" t="n"/>
+      <c r="J8" s="1" t="n"/>
+      <c r="K8" s="1" t="n"/>
+      <c r="L8" s="1" t="n"/>
+      <c r="M8" s="1" t="n"/>
+      <c r="N8" s="1" t="n"/>
+      <c r="O8" s="1" t="n"/>
+    </row>
+    <row r="9" ht="22.5" customHeight="1">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="1" t="n"/>
+      <c r="I9" s="1" t="n"/>
+      <c r="J9" s="1" t="n"/>
+      <c r="K9" s="1" t="n"/>
+      <c r="L9" s="1" t="n"/>
+      <c r="M9" s="1" t="n"/>
+      <c r="N9" s="1" t="n"/>
+      <c r="O9" s="1" t="n"/>
+    </row>
+    <row r="10" ht="22.5" customHeight="1">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
+      <c r="E10" s="1" t="n"/>
       <c r="F10" s="1" t="n"/>
       <c r="G10" s="1" t="n"/>
+      <c r="H10" s="1" t="n"/>
+      <c r="I10" s="1" t="n"/>
+      <c r="J10" s="1" t="n"/>
+      <c r="K10" s="1" t="n"/>
+      <c r="L10" s="1" t="n"/>
+      <c r="M10" s="1" t="n"/>
+      <c r="N10" s="1" t="n"/>
+      <c r="O10" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>